<commit_message>
Small things. Removed the box management tools from main view initially
</commit_message>
<xml_diff>
--- a/autosave_log_v9.xlsx
+++ b/autosave_log_v9.xlsx
@@ -25,8 +25,9 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="משה אהרן_Brody" sheetId="16" state="visible" r:id="rId16"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="דניאל_Frost" sheetId="17" state="visible" r:id="rId17"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="משה דוד_Perlstein" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Students Info" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="אליעזר הלו_Levin" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Students Info" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="21" state="visible" r:id="rId21"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -457,7 +458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -471,7 +472,7 @@
     <col width="12" customWidth="1" min="3" max="3"/>
     <col width="13.2" customWidth="1" min="4" max="4"/>
     <col width="14.4" customWidth="1" min="5" max="5"/>
-    <col width="19.2" customWidth="1" min="6" max="6"/>
+    <col width="20.4" customWidth="1" min="6" max="6"/>
     <col width="15.6" customWidth="1" min="7" max="7"/>
     <col width="25.2" customWidth="1" min="8" max="8"/>
     <col width="10.8" customWidth="1" min="9" max="9"/>
@@ -996,6 +997,178 @@
         </is>
       </c>
       <c r="I12" s="3" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-06-22T20:28:09.123709</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>2025-06-22</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>20:28:09</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>student_3</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>אליעזר הלו</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Levin</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Uneasy</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-06-22T20:29:56.881586</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>2025-06-22</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>20:29:56</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>student_2</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>מרדכי עוזר הלוי</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Sofer</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Off Task</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-06-22T20:30:04.465746</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>2025-06-22</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="inlineStr">
+        <is>
+          <t>20:30:04</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>student_6</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>דניאל</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Frost</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Off Task</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-06-23T08:36:16.438901</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>2025-06-23</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="inlineStr">
+        <is>
+          <t>08:36:16</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>student_4</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>יואל</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Fass</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Off Task</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2090,7 +2263,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W6"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2480,6 +2653,47 @@
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
       <c r="W6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-06-22 20:29:56</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Behavior</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Off Task</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3698,7 +3912,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3929,6 +4143,47 @@
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
       <c r="W3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-06-22 20:30:04</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Behavior</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Off Task</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4143,7 +4398,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4151,457 +4406,188 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="25" customWidth="1" min="5" max="5"/>
-    <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="16" customWidth="1" min="4" max="4"/>
+    <col width="28" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="40" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="12" customWidth="1" min="9" max="9"/>
+    <col width="14" customWidth="1" min="10" max="10"/>
+    <col width="19" customWidth="1" min="11" max="11"/>
+    <col width="10" customWidth="1" min="12" max="12"/>
+    <col width="13" customWidth="1" min="13" max="13"/>
+    <col width="15" customWidth="1" min="14" max="14"/>
+    <col width="13" customWidth="1" min="15" max="15"/>
+    <col width="23" customWidth="1" min="16" max="16"/>
+    <col width="10" customWidth="1" min="17" max="17"/>
+    <col width="18" customWidth="1" min="18" max="18"/>
+    <col width="23" customWidth="1" min="19" max="19"/>
+    <col width="14" customWidth="1" min="20" max="20"/>
+    <col width="18" customWidth="1" min="21" max="21"/>
+    <col width="17" customWidth="1" min="22" max="22"/>
+    <col width="19" customWidth="1" min="23" max="23"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="inlineStr">
         <is>
-          <t>Student ID</t>
+          <t>Timestamp</t>
         </is>
       </c>
       <c r="B1" s="4" t="inlineStr">
         <is>
-          <t>First Name</t>
+          <t>Type</t>
         </is>
       </c>
       <c r="C1" s="4" t="inlineStr">
         <is>
-          <t>Last Name</t>
+          <t>Behavior/Homework/Quiz Name</t>
         </is>
       </c>
       <c r="D1" s="4" t="inlineStr">
         <is>
-          <t>Nickname</t>
+          <t>Correct/Did</t>
         </is>
       </c>
       <c r="E1" s="4" t="inlineStr">
         <is>
-          <t>Full Name</t>
+          <t>Total Qs/Total Selected</t>
         </is>
       </c>
       <c r="F1" s="4" t="inlineStr">
         <is>
-          <t>Gender</t>
+          <t>Percentage</t>
         </is>
       </c>
       <c r="G1" s="4" t="inlineStr">
         <is>
-          <t>Group Name</t>
+          <t>Comment</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>Day</t>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <t>Correct</t>
+        </is>
+      </c>
+      <c r="J1" s="4" t="inlineStr">
+        <is>
+          <t>Incorrect</t>
+        </is>
+      </c>
+      <c r="K1" s="4" t="inlineStr">
+        <is>
+          <t>Partial Credit</t>
+        </is>
+      </c>
+      <c r="L1" s="4" t="inlineStr">
+        <is>
+          <t>Bonus</t>
+        </is>
+      </c>
+      <c r="M1" s="4" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="N1" s="4" t="inlineStr">
+        <is>
+          <t>Incomplete</t>
+        </is>
+      </c>
+      <c r="O1" s="4" t="inlineStr">
+        <is>
+          <t>Not Done</t>
+        </is>
+      </c>
+      <c r="P1" s="4" t="inlineStr">
+        <is>
+          <t>Effort Score (1-5)</t>
+        </is>
+      </c>
+      <c r="Q1" s="4" t="inlineStr">
+        <is>
+          <t>5gret</t>
+        </is>
+      </c>
+      <c r="R1" s="4" t="inlineStr">
+        <is>
+          <t>New Mark Type</t>
+        </is>
+      </c>
+      <c r="S1" s="4" t="inlineStr">
+        <is>
+          <t>Reading Assignment</t>
+        </is>
+      </c>
+      <c r="T1" s="4" t="inlineStr">
+        <is>
+          <t>Worksheet</t>
+        </is>
+      </c>
+      <c r="U1" s="4" t="inlineStr">
+        <is>
+          <t>Math Problems</t>
+        </is>
+      </c>
+      <c r="V1" s="4" t="inlineStr">
+        <is>
+          <t>Project Work</t>
+        </is>
+      </c>
+      <c r="W1" s="4" t="inlineStr">
+        <is>
+          <t>Study for Test</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>student_7</t>
+          <t>2025-06-22 20:28:09</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>יעקב יהושע הכהן</t>
+          <t>Behavior</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Brecher</t>
+          <t>Uneasy</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>יעקב יהושע הכהן Brecher</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Boy</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>student_9</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>משה אהרן</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Brody</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>משה אהרן Brody</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Boy</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>student_23</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>משה</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Eidelman</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>משה Eidelman</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Boy</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>student_4</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>יואל</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Fass</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>יואל Fass</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Boy</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>student_12</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>אברהם אהרן דוב</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Fogel</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>אברהם אהרן דוב Fogel</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Boy</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>student_6</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>דניאל</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Frost</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>דניאל Frost</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Boy</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>student_10</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>יצחק</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Hess</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>יצחק Hess</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Boy</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>student_18</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>אשר זעליג</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Konigsberg</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>אשר זעליג Konigsberg</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Boy</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>student_15</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>משה דוד</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Perlstein</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>משה דוד Perlstein</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Boy</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>student_26</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>משה בונים</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Rotkin</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>משה בונים Rotkin</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Boy</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>student_16</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>יעקב</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Scheinerman</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>יעקב Scheinerman</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Boy</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>student_2</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>מרדכי עוזר הלוי</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Sofer</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>מרדכי עוזר הלוי Sofer</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Boy</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>student_21</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>ברוך</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Teller</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>ברוך Teller</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Boy</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>student_24</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>ירוחם</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Tillim</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>ירוחם Tillim</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Boy</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5236,7 +5222,507 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Student ID</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Nickname</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Full Name</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>Gender</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>Group Name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>student_7</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>יעקב יהושע הכהן</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Brecher</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>יעקב יהושע הכהן Brecher</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Boy</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>student_9</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>משה אהרן</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Brody</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>משה אהרן Brody</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Boy</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>student_23</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>משה</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Eidelman</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>משה Eidelman</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Boy</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>student_4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>יואל</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Fass</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>יואל Fass</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Boy</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>student_12</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>אברהם אהרן דוב</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Fogel</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>אברהם אהרן דוב Fogel</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Boy</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>student_6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>דניאל</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Frost</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>דניאל Frost</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Boy</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>student_10</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>יצחק</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Hess</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>יצחק Hess</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Boy</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>student_18</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>אשר זעליג</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Konigsberg</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>אשר זעליג Konigsberg</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Boy</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>student_3</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>אליעזר הלו</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Levin</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>אליעזר הלו Levin</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Boy</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>student_15</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>משה דוד</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Perlstein</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>משה דוד Perlstein</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Boy</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>student_26</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>משה בונים</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Rotkin</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>משה בונים Rotkin</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Boy</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>student_16</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>יעקב</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Scheinerman</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>יעקב Scheinerman</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Boy</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>student_2</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>מרדכי עוזר הלוי</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Sofer</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>מרדכי עוזר הלוי Sofer</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Boy</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>student_21</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ברוך</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Teller</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>ברוך Teller</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Boy</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>student_24</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ירוחם</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Tillim</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>ירוחם Tillim</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Boy</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5323,7 +5809,7 @@
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -5368,7 +5854,7 @@
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -5404,7 +5890,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>משה בונים Rotkin</t>
+          <t>אליעזר הלו Levin</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -5419,12 +5905,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>יעקב Scheinerman</t>
+          <t>משה בונים Rotkin</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Fighting</t>
+          <t>Uneasy</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -5434,91 +5920,81 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ברוך Teller</t>
+          <t>יעקב Scheinerman</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Uneasy</t>
+          <t>Fighting</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
         <v>1</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>מרדכי עוזר הלוי Sofer</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Off Task</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
     <row r="17">
-      <c r="A17" s="6" t="inlineStr">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ברוך Teller</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Uneasy</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="inlineStr">
         <is>
           <t>Quiz Averages by Student</t>
         </is>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="7" t="inlineStr">
+    <row r="20">
+      <c r="A20" s="7" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="B18" s="7" t="inlineStr">
+      <c r="B20" s="7" t="inlineStr">
         <is>
           <t>Quiz Name</t>
         </is>
       </c>
-      <c r="C18" s="7" t="inlineStr">
+      <c r="C20" s="7" t="inlineStr">
         <is>
           <t>Avg Score (%)</t>
         </is>
       </c>
-      <c r="D18" s="7" t="inlineStr">
+      <c r="D20" s="7" t="inlineStr">
         <is>
           <t>Times Taken</t>
         </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>יעקב יהושע הכהן Brecher</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Pop Quiz</t>
-        </is>
-      </c>
-      <c r="C19" s="2" t="inlineStr">
-        <is>
-          <t>82.00%</t>
-        </is>
-      </c>
-      <c r="D19" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>יואל Fass</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Pop Quiz</t>
-        </is>
-      </c>
-      <c r="C20" s="2" t="inlineStr">
-        <is>
-          <t>33.00%</t>
-        </is>
-      </c>
-      <c r="D20" s="2" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>אברהם אהרן דוב Fogel</t>
+          <t>יעקב יהושע הכהן Brecher</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -5528,7 +6004,7 @@
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>82.00%</t>
         </is>
       </c>
       <c r="D21" s="2" t="n">
@@ -5538,7 +6014,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>אשר זעליג Konigsberg</t>
+          <t>יואל Fass</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -5548,7 +6024,7 @@
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>33.00%</t>
         </is>
       </c>
       <c r="D22" s="2" t="n">
@@ -5558,7 +6034,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>משה בונים Rotkin</t>
+          <t>אברהם אהרן דוב Fogel</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -5578,7 +6054,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>מרדכי עוזר הלוי Sofer</t>
+          <t>אשר זעליג Konigsberg</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -5598,7 +6074,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>ברוך Teller</t>
+          <t>משה בונים Rotkin</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -5618,7 +6094,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ירוחם Tillim</t>
+          <t>מרדכי עוזר הלוי Sofer</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -5635,66 +6111,74 @@
         <v>1</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>ברוך Teller</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Pop Quiz</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
     <row r="28">
-      <c r="A28" s="6" t="inlineStr">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>ירוחם Tillim</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Pop Quiz</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="inlineStr">
         <is>
           <t>Homework Completion by Student</t>
         </is>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="7" t="inlineStr">
+    <row r="31">
+      <c r="A31" s="7" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="B29" s="7" t="inlineStr">
+      <c r="B31" s="7" t="inlineStr">
         <is>
           <t>Homework Type/Session</t>
         </is>
       </c>
-      <c r="C29" s="7" t="inlineStr">
+      <c r="C31" s="7" t="inlineStr">
         <is>
           <t>Count</t>
         </is>
       </c>
-      <c r="D29" s="7" t="inlineStr">
+      <c r="D31" s="7" t="inlineStr">
         <is>
           <t>Total Points (if applicable)</t>
         </is>
       </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>יעקב יהושע הכהן Brecher</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="C30" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D30" s="2" t="inlineStr"/>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>יעקב יהושע הכהן Brecher</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Excellent Work</t>
-        </is>
-      </c>
-      <c r="C31" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D31" s="2" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -5704,17 +6188,13 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Homework Check</t>
+          <t>Done</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D32" s="2" t="inlineStr">
-        <is>
-          <t>10.00</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D32" s="2" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -5724,7 +6204,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Homework Check2</t>
+          <t>Excellent Work</t>
         </is>
       </c>
       <c r="C33" s="2" t="n">
@@ -5740,11 +6220,11 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Reading Assignment</t>
+          <t>Homework Check</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D34" s="2" t="inlineStr">
         <is>
@@ -5755,12 +6235,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>יואל Fass</t>
+          <t>יעקב יהושע הכהן Brecher</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Homework Check</t>
+          <t>Homework Check2</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
@@ -5771,12 +6251,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>אברהם אהרן דוב Fogel</t>
+          <t>יעקב יהושע הכהן Brecher</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Done</t>
+          <t>Reading Assignment</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
@@ -5784,14 +6264,14 @@
       </c>
       <c r="D36" s="2" t="inlineStr">
         <is>
-          <t>12.00</t>
+          <t>10.00</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>אברהם אהרן דוב Fogel</t>
+          <t>יואל Fass</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -5800,13 +6280,9 @@
         </is>
       </c>
       <c r="C37" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D37" s="2" t="inlineStr">
-        <is>
-          <t>30.00</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D37" s="2" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -5816,13 +6292,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Homework Check2</t>
+          <t>Done</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D38" s="2" t="inlineStr"/>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>12.00</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -5832,15 +6312,15 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Project Work</t>
+          <t>Homework Check</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D39" s="2" t="inlineStr">
         <is>
-          <t>70.00</t>
+          <t>30.00</t>
         </is>
       </c>
     </row>
@@ -5852,7 +6332,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Worksheet</t>
+          <t>Homework Check2</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
@@ -5863,7 +6343,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>יצחק Hess</t>
+          <t>אברהם אהרן דוב Fogel</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -5874,37 +6354,37 @@
       <c r="C41" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D41" s="2" t="inlineStr"/>
+      <c r="D41" s="2" t="inlineStr">
+        <is>
+          <t>70.00</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>אשר זעליג Konigsberg</t>
+          <t>אברהם אהרן דוב Fogel</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Homework Check</t>
+          <t>Worksheet</t>
         </is>
       </c>
       <c r="C42" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D42" s="2" t="inlineStr">
-        <is>
-          <t>10.00</t>
-        </is>
-      </c>
+      <c r="D42" s="2" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>אשר זעליג Konigsberg</t>
+          <t>יצחק Hess</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Homework Check2</t>
+          <t>Project Work</t>
         </is>
       </c>
       <c r="C43" s="2" t="n">
@@ -5915,48 +6395,48 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>משה דוד Perlstein</t>
+          <t>אשר זעליג Konigsberg</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Worksheet</t>
+          <t>Homework Check</t>
         </is>
       </c>
       <c r="C44" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D44" s="2" t="inlineStr"/>
+      <c r="D44" s="2" t="inlineStr">
+        <is>
+          <t>10.00</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>משה בונים Rotkin</t>
+          <t>אשר זעליג Konigsberg</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Homework Check</t>
+          <t>Homework Check2</t>
         </is>
       </c>
       <c r="C45" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D45" s="2" t="inlineStr">
-        <is>
-          <t>30.00</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D45" s="2" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>משה בונים Rotkin</t>
+          <t>משה דוד Perlstein</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Homework Check2</t>
+          <t>Worksheet</t>
         </is>
       </c>
       <c r="C46" s="2" t="n">
@@ -5972,13 +6452,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Project Work</t>
+          <t>Homework Check</t>
         </is>
       </c>
       <c r="C47" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D47" s="2" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="D47" s="2" t="inlineStr">
+        <is>
+          <t>30.00</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -5988,7 +6472,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Homework Check2</t>
         </is>
       </c>
       <c r="C48" s="2" t="n">
@@ -5999,12 +6483,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>מרדכי עוזר הלוי Sofer</t>
+          <t>משה בונים Rotkin</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Done</t>
+          <t>Project Work</t>
         </is>
       </c>
       <c r="C49" s="2" t="n">
@@ -6015,16 +6499,16 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>מרדכי עוזר הלוי Sofer</t>
+          <t>משה בונים Rotkin</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Homework Check</t>
+          <t>gt</t>
         </is>
       </c>
       <c r="C50" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D50" s="2" t="inlineStr"/>
     </row>
@@ -6036,7 +6520,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Homework Check2</t>
+          <t>Done</t>
         </is>
       </c>
       <c r="C51" s="2" t="n">
@@ -6047,48 +6531,44 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>ברוך Teller</t>
+          <t>מרדכי עוזר הלוי Sofer</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Excellent Work</t>
+          <t>Homework Check</t>
         </is>
       </c>
       <c r="C52" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D52" s="2" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>ברוך Teller</t>
+          <t>מרדכי עוזר הלוי Sofer</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Homework Check</t>
+          <t>Homework Check2</t>
         </is>
       </c>
       <c r="C53" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D53" s="2" t="inlineStr">
-        <is>
-          <t>30.00</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D53" s="2" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>ירוחם Tillim</t>
+          <t>ברוך Teller</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Homework Check2</t>
+          <t>Excellent Work</t>
         </is>
       </c>
       <c r="C54" s="2" t="n">
@@ -6099,18 +6579,54 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
+          <t>ברוך Teller</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Homework Check</t>
+        </is>
+      </c>
+      <c r="C55" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D55" s="2" t="inlineStr">
+        <is>
+          <t>30.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
           <t>ירוחם Tillim</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Homework Check2</t>
+        </is>
+      </c>
+      <c r="C56" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D56" s="2" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>ירוחם Tillim</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
         <is>
           <t>Late</t>
         </is>
       </c>
-      <c r="C55" s="2" t="n">
+      <c r="C57" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D55" s="2" t="inlineStr"/>
+      <c r="D57" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8003,7 +8519,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF52"/>
+  <dimension ref="A1:AF56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -11155,6 +11671,198 @@
       <c r="AF52" t="inlineStr">
         <is>
           <t>Homework</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2025-06-22T20:28:09.123709</t>
+        </is>
+      </c>
+      <c r="B53" s="2" t="inlineStr">
+        <is>
+          <t>2025-06-22</t>
+        </is>
+      </c>
+      <c r="C53" s="2" t="inlineStr">
+        <is>
+          <t>20:28:09</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>student_3</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>אליעזר הלו</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Levin</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Uneasy</t>
+        </is>
+      </c>
+      <c r="AE53" s="3" t="inlineStr"/>
+      <c r="AF53" t="inlineStr">
+        <is>
+          <t>Behavior</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-06-22T20:29:56.881586</t>
+        </is>
+      </c>
+      <c r="B54" s="2" t="inlineStr">
+        <is>
+          <t>2025-06-22</t>
+        </is>
+      </c>
+      <c r="C54" s="2" t="inlineStr">
+        <is>
+          <t>20:29:56</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>student_2</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>מרדכי עוזר הלוי</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Sofer</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Off Task</t>
+        </is>
+      </c>
+      <c r="AE54" s="3" t="inlineStr"/>
+      <c r="AF54" t="inlineStr">
+        <is>
+          <t>Behavior</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2025-06-22T20:30:04.465746</t>
+        </is>
+      </c>
+      <c r="B55" s="2" t="inlineStr">
+        <is>
+          <t>2025-06-22</t>
+        </is>
+      </c>
+      <c r="C55" s="2" t="inlineStr">
+        <is>
+          <t>20:30:04</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>student_6</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>דניאל</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Frost</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>Off Task</t>
+        </is>
+      </c>
+      <c r="AE55" s="3" t="inlineStr"/>
+      <c r="AF55" t="inlineStr">
+        <is>
+          <t>Behavior</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2025-06-23T08:36:16.438901</t>
+        </is>
+      </c>
+      <c r="B56" s="2" t="inlineStr">
+        <is>
+          <t>2025-06-23</t>
+        </is>
+      </c>
+      <c r="C56" s="2" t="inlineStr">
+        <is>
+          <t>08:36:16</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>student_4</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>יואל</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Fass</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>Off Task</t>
+        </is>
+      </c>
+      <c r="AE56" s="3" t="inlineStr"/>
+      <c r="AF56" t="inlineStr">
+        <is>
+          <t>Behavior</t>
         </is>
       </c>
     </row>
@@ -11371,7 +12079,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11714,6 +12422,47 @@
       <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
       <c r="W5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-06-23 08:36:16</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Behavior</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Off Task</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>